<commit_message>
change 24 hours time format to 12 hours format
</commit_message>
<xml_diff>
--- a/public/assets/sample-guard-roaster/guard-roaster.xlsx
+++ b/public/assets/sample-guard-roaster/guard-roaster.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="74">
   <si>
     <t>guard_id</t>
   </si>
@@ -57,6 +57,198 @@
   </si>
   <si>
     <t>time_out</t>
+  </si>
+  <si>
+    <t>9:30AM</t>
+  </si>
+  <si>
+    <t>12:10PM</t>
+  </si>
+  <si>
+    <t>12:00AM</t>
+  </si>
+  <si>
+    <t>5:48PM</t>
+  </si>
+  <si>
+    <t>5:40AM</t>
+  </si>
+  <si>
+    <t>5:41AM</t>
+  </si>
+  <si>
+    <t>5:42PM</t>
+  </si>
+  <si>
+    <t>5:43AM</t>
+  </si>
+  <si>
+    <t>5:44PM</t>
+  </si>
+  <si>
+    <t>12:30PM</t>
+  </si>
+  <si>
+    <t>9:00AM</t>
+  </si>
+  <si>
+    <t>9:31AM</t>
+  </si>
+  <si>
+    <t>12:01AM</t>
+  </si>
+  <si>
+    <t>9:40AM</t>
+  </si>
+  <si>
+    <t>5:40PM</t>
+  </si>
+  <si>
+    <t>5:49PM</t>
+  </si>
+  <si>
+    <t>5:42AM</t>
+  </si>
+  <si>
+    <t>3:32PM</t>
+  </si>
+  <si>
+    <t>5:44AM</t>
+  </si>
+  <si>
+    <t>5:45AM</t>
+  </si>
+  <si>
+    <t>4:30AM</t>
+  </si>
+  <si>
+    <t>9:32AM</t>
+  </si>
+  <si>
+    <t>12:02AM</t>
+  </si>
+  <si>
+    <t>9:41AM</t>
+  </si>
+  <si>
+    <t>5:41PM</t>
+  </si>
+  <si>
+    <t>5:50PM</t>
+  </si>
+  <si>
+    <t>3:33PM</t>
+  </si>
+  <si>
+    <t>5:46AM</t>
+  </si>
+  <si>
+    <t>5:30AM</t>
+  </si>
+  <si>
+    <t>12:31PM</t>
+  </si>
+  <si>
+    <t>9:33AM</t>
+  </si>
+  <si>
+    <t>12:03AM</t>
+  </si>
+  <si>
+    <t>9:42AM</t>
+  </si>
+  <si>
+    <t>5:51PM</t>
+  </si>
+  <si>
+    <t>3:34PM</t>
+  </si>
+  <si>
+    <t>5:47AM</t>
+  </si>
+  <si>
+    <t>5:31AM</t>
+  </si>
+  <si>
+    <t>12:32PM</t>
+  </si>
+  <si>
+    <t>9:34AM</t>
+  </si>
+  <si>
+    <t>12:04AM</t>
+  </si>
+  <si>
+    <t>9:43AM</t>
+  </si>
+  <si>
+    <t>5:43PM</t>
+  </si>
+  <si>
+    <t>5:52PM</t>
+  </si>
+  <si>
+    <t>3:35PM</t>
+  </si>
+  <si>
+    <t>5:48AM</t>
+  </si>
+  <si>
+    <t>5:32AM</t>
+  </si>
+  <si>
+    <t>12:33PM</t>
+  </si>
+  <si>
+    <t>9:35AM</t>
+  </si>
+  <si>
+    <t>12:05AM</t>
+  </si>
+  <si>
+    <t>9:44AM</t>
+  </si>
+  <si>
+    <t>5:53PM</t>
+  </si>
+  <si>
+    <t>3:36PM</t>
+  </si>
+  <si>
+    <t>5:78PM</t>
+  </si>
+  <si>
+    <t>5:49AM</t>
+  </si>
+  <si>
+    <t>5:33AM</t>
+  </si>
+  <si>
+    <t>12:34PM</t>
+  </si>
+  <si>
+    <t>9:36AM</t>
+  </si>
+  <si>
+    <t>12:06AM</t>
+  </si>
+  <si>
+    <t>9:45AM</t>
+  </si>
+  <si>
+    <t>5:45PM</t>
+  </si>
+  <si>
+    <t>5:54PM</t>
+  </si>
+  <si>
+    <t>3:37PM</t>
+  </si>
+  <si>
+    <t>5:79PM</t>
+  </si>
+  <si>
+    <t>5:50AM</t>
   </si>
 </sst>
 </file>
@@ -1218,10 +1410,13 @@
   <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <cols>
+    <col min="5" max="5" width="9.85714285714286" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
@@ -1295,40 +1490,42 @@
     </row>
     <row r="3" spans="1:14">
       <c r="A3">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3" s="2">
-        <v>0.375</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0.6875</v>
-      </c>
-      <c r="E3" s="2">
-        <v>0.395833333333333</v>
-      </c>
-      <c r="F3" s="2">
-        <v>0.708333333333333</v>
-      </c>
-      <c r="G3" s="2">
-        <v>0.383333333333333</v>
-      </c>
-      <c r="H3" s="2">
-        <v>0.75</v>
-      </c>
-      <c r="I3" s="2">
-        <v>0.166666666666667</v>
-      </c>
-      <c r="J3" s="2">
-        <v>0.791666666666667</v>
-      </c>
-      <c r="M3" s="2">
-        <v>0.322916666666667</v>
-      </c>
-      <c r="N3" s="2">
-        <v>0.708333333333333</v>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -1338,41 +1535,41 @@
       <c r="B4">
         <v>2</v>
       </c>
-      <c r="C4" s="2">
-        <v>0.416666666666667</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0.729166666666667</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0.4375</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0.75</v>
-      </c>
-      <c r="G4" s="2">
-        <v>0.425</v>
-      </c>
-      <c r="H4" s="2">
-        <v>0.791666666666667</v>
-      </c>
-      <c r="I4" s="2">
-        <v>0.208333333333333</v>
-      </c>
-      <c r="J4" s="2">
-        <v>0.833333333333333</v>
-      </c>
-      <c r="K4" s="2">
-        <v>0.0833333333333333</v>
-      </c>
-      <c r="L4" s="2">
-        <v>0.239583333333333</v>
-      </c>
-      <c r="M4" s="2">
-        <v>0.364583333333333</v>
-      </c>
-      <c r="N4" s="2">
-        <v>0.75</v>
+      <c r="C4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -1382,211 +1579,211 @@
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5" s="2">
-        <v>0.458333333333333</v>
-      </c>
-      <c r="D5" s="2">
-        <v>0.770833333333333</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0.479166666666667</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0.791666666666667</v>
-      </c>
-      <c r="G5" s="2">
-        <v>0.466666666666667</v>
-      </c>
-      <c r="H5" s="2">
-        <v>0.833333333333333</v>
-      </c>
-      <c r="I5" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="J5" s="2">
-        <v>0.875</v>
-      </c>
-      <c r="K5" s="2">
-        <v>0.125</v>
-      </c>
-      <c r="L5" s="2">
-        <v>0.28125</v>
-      </c>
-      <c r="M5" s="2">
-        <v>0.40625</v>
-      </c>
-      <c r="N5" s="2">
-        <v>0.791666666666667</v>
+      <c r="C5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>2</v>
       </c>
-      <c r="C6" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="D6" s="2">
-        <v>0.8125</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0.520833333333333</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0.833333333333333</v>
-      </c>
-      <c r="G6" s="2">
-        <v>0.508333333333333</v>
-      </c>
-      <c r="H6" s="2">
-        <v>0.833333333333333</v>
-      </c>
-      <c r="I6" s="2">
-        <v>0.291666666666667</v>
-      </c>
-      <c r="J6" s="2">
-        <v>0.916666666666667</v>
-      </c>
-      <c r="K6" s="2">
-        <v>0.166666666666667</v>
-      </c>
-      <c r="L6" s="2">
-        <v>0.322916666666667</v>
-      </c>
-      <c r="M6" s="2">
-        <v>0.447916666666667</v>
-      </c>
-      <c r="N6" s="2">
-        <v>0.833333333333333</v>
+      <c r="C6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="2:14">
       <c r="B7">
         <v>1</v>
       </c>
-      <c r="C7" s="2">
-        <v>0.541666666666667</v>
-      </c>
-      <c r="D7" s="2">
-        <v>0.854166666666667</v>
-      </c>
-      <c r="E7" s="2">
-        <v>0.5625</v>
-      </c>
-      <c r="F7" s="2">
-        <v>0.875</v>
-      </c>
-      <c r="G7" s="2">
-        <v>0.55</v>
-      </c>
-      <c r="H7" s="2">
-        <v>0.875</v>
-      </c>
-      <c r="I7" s="2">
-        <v>0.208333333333333</v>
-      </c>
-      <c r="J7" s="2">
-        <v>0.958333333333333</v>
-      </c>
-      <c r="K7" s="2">
-        <v>0.208333333333333</v>
-      </c>
-      <c r="L7" s="2">
-        <v>0.28125</v>
-      </c>
-      <c r="M7" s="2">
-        <v>0.489583333333333</v>
-      </c>
-      <c r="N7" s="2">
-        <v>0.875</v>
+      <c r="C7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="2:14">
       <c r="B8">
         <v>3</v>
       </c>
-      <c r="C8" s="2">
-        <v>0.583333333333333</v>
-      </c>
-      <c r="D8" s="2">
-        <v>0.895833333333333</v>
-      </c>
-      <c r="E8" s="2">
-        <v>0.604166666666667</v>
-      </c>
-      <c r="F8" s="2">
-        <v>0.916666666666667</v>
-      </c>
-      <c r="G8" s="2">
-        <v>0.591666666666667</v>
-      </c>
-      <c r="H8" s="2">
-        <v>0.916666666666667</v>
-      </c>
-      <c r="I8" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="J8" s="2">
-        <v>1</v>
-      </c>
-      <c r="K8" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="L8" s="2">
-        <v>0.322916666666667</v>
-      </c>
-      <c r="M8" s="2">
-        <v>0.53125</v>
-      </c>
-      <c r="N8" s="2">
-        <v>0.916666666666667</v>
+      <c r="C8" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:14">
       <c r="A9">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B9">
         <v>3</v>
       </c>
-      <c r="C9" s="2">
-        <v>0.541666666666667</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0.9375</v>
-      </c>
-      <c r="E9" s="2">
-        <v>0.645833333333333</v>
-      </c>
-      <c r="F9" s="2">
-        <v>0.958333333333333</v>
-      </c>
-      <c r="G9" s="2">
-        <v>0.633333333333333</v>
-      </c>
-      <c r="H9" s="2">
-        <v>0.958333333333333</v>
-      </c>
-      <c r="I9" s="2">
-        <v>0.291666666666667</v>
-      </c>
-      <c r="J9" s="2">
-        <v>1.04166666666667</v>
-      </c>
-      <c r="K9" s="2">
-        <v>0.291666666666667</v>
-      </c>
-      <c r="L9" s="2">
-        <v>0.364583333333333</v>
-      </c>
-      <c r="M9" s="2">
-        <v>0.572916666666667</v>
-      </c>
-      <c r="N9" s="2">
-        <v>0.958333333333333</v>
+      <c r="C9" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>